<commit_message>
Excel VBA formatando com recurso de tabela
</commit_message>
<xml_diff>
--- a/Projeto loja de sapatos  1.xlsx
+++ b/Projeto loja de sapatos  1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clebe\OneDrive\Documentos\Curso Excel-VBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D713FD3-0983-48B5-83FA-741D7B40AAB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6BA250-0065-4565-9B88-D0B700D9D873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-75" windowWidth="15600" windowHeight="11160" xr2:uid="{676D38EB-A95E-4CBE-87C2-02F68F25127A}"/>
   </bookViews>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
-  <si>
-    <t>tenis inafantil vermellho</t>
-  </si>
-  <si>
-    <t>tenis infantil  azul</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t xml:space="preserve">tenis infantil  rosa </t>
   </si>
@@ -56,23 +50,29 @@
     <t>Tamanho</t>
   </si>
   <si>
-    <t>tenis  infantil azul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tenis infantil azul </t>
-  </si>
-  <si>
-    <t>tenis adulto masculino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tenis adulto feminino </t>
+    <t>tenis adulto feminino</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tenis infantil  vermelho </t>
+  </si>
+  <si>
+    <t>tenis infantil azul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tenis infantil rosa </t>
+  </si>
+  <si>
+    <t>vans autentico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,16 +80,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -97,12 +117,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,119 +465,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BB1467-CC0B-4592-ADCF-1A2BD97E2DA2}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B12" s="4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel VBA conhecendo os formatos de guia
</commit_message>
<xml_diff>
--- a/Projeto loja de sapatos  1.xlsx
+++ b/Projeto loja de sapatos  1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clebe\OneDrive\Documentos\Curso Excel-VBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6BA250-0065-4565-9B88-D0B700D9D873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8120D21E-8B1E-4EA2-B2D1-43E8F1CCE155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-75" windowWidth="15600" windowHeight="11160" xr2:uid="{676D38EB-A95E-4CBE-87C2-02F68F25127A}"/>
   </bookViews>
@@ -33,23 +33,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t xml:space="preserve">tenis infantil  rosa </t>
   </si>
   <si>
-    <t>Produtos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sapato social feminino </t>
   </si>
   <si>
     <t xml:space="preserve">Sapato social masculino </t>
   </si>
   <si>
-    <t>Tamanho</t>
-  </si>
-  <si>
     <t>tenis adulto feminino</t>
   </si>
   <si>
@@ -66,13 +60,22 @@
   </si>
   <si>
     <t>vans autentico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lista de produtos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrição </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamanho </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,9 +84,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="7" tint="0.59999389629810485"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,18 +123,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,20 +147,7 @@
         <color theme="4" tint="0.39997558519241921"/>
       </left>
       <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -143,14 +155,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,156 +496,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3BB1467-CC0B-4592-ADCF-1A2BD97E2DA2}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="11">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="11">
+        <v>42</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B16" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="6">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="6">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="6">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="4">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="4">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>6</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
estudando Excel Vba - proejto controle de estoque de uma loja de tenis
</commit_message>
<xml_diff>
--- a/Projeto loja de sapatos  1.xlsx
+++ b/Projeto loja de sapatos  1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clebe\OneDrive\Documentos\Curso Excel-VBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clebe\OneDrive\Documentos\Excel VBA - Alura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE44728-D000-4FE0-8707-158CF720D551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091A7008-19DC-4B18-988D-BB8A71E8E88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-75" windowWidth="15600" windowHeight="11160" xr2:uid="{676D38EB-A95E-4CBE-87C2-02F68F25127A}"/>
   </bookViews>
@@ -33,29 +33,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">tenis infantil  rosa </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">tenis infantil  vermelho </t>
-  </si>
-  <si>
-    <t>tenis infantil azul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tenis infantil rosa </t>
-  </si>
-  <si>
     <t>vans autentico</t>
   </si>
   <si>
-    <t xml:space="preserve">lista de produtos </t>
-  </si>
-  <si>
     <t xml:space="preserve">Descrição </t>
   </si>
   <si>
@@ -77,13 +62,31 @@
     <t xml:space="preserve">chinelo adidas </t>
   </si>
   <si>
-    <t xml:space="preserve"> Preço</t>
+    <t>Preço</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tenis de corrida </t>
+  </si>
+  <si>
+    <t xml:space="preserve">havaianas na cor  branca </t>
+  </si>
+  <si>
+    <t xml:space="preserve">adidas masculino casual </t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controle de estoque Loja de tenis </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -138,12 +141,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -153,24 +156,71 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -179,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -189,22 +239,40 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -524,7 +592,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,172 +604,207 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12"/>
+      <c r="A1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6">
+        <v>25</v>
+      </c>
+      <c r="C3" s="12">
+        <v>45.5</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6">
+        <v>32</v>
+      </c>
+      <c r="C4" s="12">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6">
+        <v>35</v>
+      </c>
+      <c r="C5" s="12">
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6">
+        <v>25</v>
+      </c>
+      <c r="C6" s="12">
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="6">
+        <v>32</v>
+      </c>
+      <c r="C7" s="12">
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6">
+        <v>35</v>
+      </c>
+      <c r="C8" s="12">
+        <v>80.5</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6">
+        <v>25</v>
+      </c>
+      <c r="C9" s="12">
+        <v>150.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="6">
+        <v>32</v>
+      </c>
+      <c r="C10" s="12">
+        <v>150.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="6">
+        <v>35</v>
+      </c>
+      <c r="C11" s="12">
+        <v>150.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6">
+        <v>40</v>
+      </c>
+      <c r="C12" s="12">
+        <v>270.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="6">
+        <v>42</v>
+      </c>
+      <c r="C13" s="12">
+        <v>550.20000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="6">
+        <v>41</v>
+      </c>
+      <c r="C14" s="12">
+        <v>1500.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="6">
+        <v>42</v>
+      </c>
+      <c r="C15" s="12">
+        <v>1500.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B16" s="6">
+        <v>45</v>
+      </c>
+      <c r="C16" s="12">
+        <v>350.65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8">
-        <v>25</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8">
-        <v>32</v>
-      </c>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="8">
-        <v>35</v>
-      </c>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8">
-        <v>25</v>
-      </c>
-      <c r="C6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="8">
-        <v>32</v>
-      </c>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="8">
-        <v>35</v>
-      </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="8">
-        <v>25</v>
-      </c>
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="8">
-        <v>32</v>
-      </c>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="8">
-        <v>35</v>
-      </c>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="8">
-        <v>40</v>
-      </c>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="8">
-        <v>42</v>
-      </c>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="8">
-        <v>41</v>
-      </c>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="8">
-        <v>42</v>
-      </c>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="8">
-        <v>45</v>
-      </c>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="B17" s="14">
+        <v>38</v>
+      </c>
+      <c r="C17" s="15">
+        <v>175.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="8">
-        <v>38</v>
-      </c>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
+      <c r="C18" s="18">
+        <f>SUM(C3:C17)</f>
+        <v>5180.1999999999989</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F21" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>